<commit_message>
removed some old variables related to soil carbon.
</commit_message>
<xml_diff>
--- a/ref/preliminary_calibration_info/df_af_var_calib.xlsx
+++ b/ref/preliminary_calibration_info/df_af_var_calib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/preliminary_calibration_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183B48FF-4D2E-C642-BF3B-714182FC7394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A05B9D-3885-2B45-9D5B-D332A02AA365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="460" windowWidth="35840" windowHeight="20040" xr2:uid="{C56D6200-D790-8F41-83C3-9FCF52DEFC0A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="621">
   <si>
     <t>Agriculture</t>
   </si>
@@ -1959,6 +1959,9 @@
   </si>
   <si>
     <t>All gnrl variables should be the same for all sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emission factors for land use conversion are based on Costa Rica's relative values. They should be scaled up/down collectively. </t>
   </si>
 </sst>
 </file>
@@ -2457,7 +2460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2620,6 +2623,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2938,9 +2944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C64BE5-C8DA-C44F-8D4A-1132CA069F94}">
   <dimension ref="A1:V572"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F224" sqref="F224:H273"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V165" sqref="V165:V228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6993,7 +6999,9 @@
       </c>
       <c r="E165"/>
       <c r="H165" s="1"/>
-      <c r="V165" s="58"/>
+      <c r="V165" s="62" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="166" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
@@ -7010,7 +7018,7 @@
       </c>
       <c r="E166"/>
       <c r="H166" s="1"/>
-      <c r="V166" s="58"/>
+      <c r="V166" s="62"/>
     </row>
     <row r="167" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
@@ -7027,7 +7035,7 @@
       </c>
       <c r="E167"/>
       <c r="H167" s="1"/>
-      <c r="V167" s="58"/>
+      <c r="V167" s="62"/>
     </row>
     <row r="168" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
@@ -7044,7 +7052,7 @@
       </c>
       <c r="E168"/>
       <c r="H168" s="1"/>
-      <c r="V168" s="58"/>
+      <c r="V168" s="62"/>
     </row>
     <row r="169" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
@@ -7061,7 +7069,7 @@
       </c>
       <c r="E169"/>
       <c r="H169" s="1"/>
-      <c r="V169" s="58"/>
+      <c r="V169" s="62"/>
     </row>
     <row r="170" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
@@ -7078,7 +7086,7 @@
       </c>
       <c r="E170"/>
       <c r="H170" s="1"/>
-      <c r="V170" s="58"/>
+      <c r="V170" s="62"/>
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
@@ -7095,7 +7103,7 @@
       </c>
       <c r="E171"/>
       <c r="H171" s="1"/>
-      <c r="V171" s="58"/>
+      <c r="V171" s="62"/>
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
@@ -7112,7 +7120,7 @@
       </c>
       <c r="E172"/>
       <c r="H172" s="1"/>
-      <c r="V172" s="58"/>
+      <c r="V172" s="62"/>
     </row>
     <row r="173" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
@@ -7129,7 +7137,7 @@
       </c>
       <c r="E173"/>
       <c r="H173" s="1"/>
-      <c r="V173" s="58"/>
+      <c r="V173" s="62"/>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
@@ -7146,7 +7154,7 @@
       </c>
       <c r="E174"/>
       <c r="H174" s="1"/>
-      <c r="V174" s="58"/>
+      <c r="V174" s="62"/>
     </row>
     <row r="175" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
@@ -7163,7 +7171,7 @@
       </c>
       <c r="E175"/>
       <c r="H175" s="1"/>
-      <c r="V175" s="58"/>
+      <c r="V175" s="62"/>
     </row>
     <row r="176" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
@@ -7180,7 +7188,7 @@
       </c>
       <c r="E176"/>
       <c r="H176" s="1"/>
-      <c r="V176" s="58"/>
+      <c r="V176" s="62"/>
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
@@ -7197,7 +7205,7 @@
       </c>
       <c r="E177"/>
       <c r="H177" s="1"/>
-      <c r="V177" s="58"/>
+      <c r="V177" s="62"/>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
@@ -7214,7 +7222,7 @@
       </c>
       <c r="E178"/>
       <c r="H178" s="1"/>
-      <c r="V178" s="58"/>
+      <c r="V178" s="62"/>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
@@ -7231,7 +7239,7 @@
       </c>
       <c r="E179"/>
       <c r="H179" s="1"/>
-      <c r="V179" s="58"/>
+      <c r="V179" s="62"/>
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
@@ -7248,7 +7256,7 @@
       </c>
       <c r="E180"/>
       <c r="H180" s="1"/>
-      <c r="V180" s="58"/>
+      <c r="V180" s="62"/>
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
@@ -7265,7 +7273,7 @@
       </c>
       <c r="E181"/>
       <c r="H181" s="1"/>
-      <c r="V181" s="58"/>
+      <c r="V181" s="62"/>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
@@ -7282,7 +7290,7 @@
       </c>
       <c r="E182"/>
       <c r="H182" s="1"/>
-      <c r="V182" s="58"/>
+      <c r="V182" s="62"/>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
@@ -7299,7 +7307,7 @@
       </c>
       <c r="E183"/>
       <c r="H183" s="1"/>
-      <c r="V183" s="58"/>
+      <c r="V183" s="62"/>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
@@ -7316,7 +7324,7 @@
       </c>
       <c r="E184"/>
       <c r="H184" s="1"/>
-      <c r="V184" s="58"/>
+      <c r="V184" s="62"/>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
@@ -7333,7 +7341,7 @@
       </c>
       <c r="E185"/>
       <c r="H185" s="1"/>
-      <c r="V185" s="58"/>
+      <c r="V185" s="62"/>
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
@@ -7350,7 +7358,7 @@
       </c>
       <c r="E186"/>
       <c r="H186" s="1"/>
-      <c r="V186" s="58"/>
+      <c r="V186" s="62"/>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
@@ -7367,7 +7375,7 @@
       </c>
       <c r="E187"/>
       <c r="H187" s="1"/>
-      <c r="V187" s="58"/>
+      <c r="V187" s="62"/>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
@@ -7384,7 +7392,7 @@
       </c>
       <c r="E188"/>
       <c r="H188" s="1"/>
-      <c r="V188" s="58"/>
+      <c r="V188" s="62"/>
     </row>
     <row r="189" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
@@ -7401,7 +7409,7 @@
       </c>
       <c r="E189"/>
       <c r="H189" s="1"/>
-      <c r="V189" s="58"/>
+      <c r="V189" s="62"/>
     </row>
     <row r="190" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
@@ -7418,7 +7426,7 @@
       </c>
       <c r="E190"/>
       <c r="H190" s="1"/>
-      <c r="V190" s="58"/>
+      <c r="V190" s="62"/>
     </row>
     <row r="191" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
@@ -7435,7 +7443,7 @@
       </c>
       <c r="E191"/>
       <c r="H191" s="1"/>
-      <c r="V191" s="58"/>
+      <c r="V191" s="62"/>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
@@ -7452,7 +7460,7 @@
       </c>
       <c r="E192"/>
       <c r="H192" s="1"/>
-      <c r="V192" s="58"/>
+      <c r="V192" s="62"/>
     </row>
     <row r="193" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
@@ -7469,7 +7477,7 @@
       </c>
       <c r="E193"/>
       <c r="H193" s="1"/>
-      <c r="V193" s="58"/>
+      <c r="V193" s="62"/>
     </row>
     <row r="194" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
@@ -7486,7 +7494,7 @@
       </c>
       <c r="E194"/>
       <c r="H194" s="1"/>
-      <c r="V194" s="58"/>
+      <c r="V194" s="62"/>
     </row>
     <row r="195" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
@@ -7503,7 +7511,7 @@
       </c>
       <c r="E195"/>
       <c r="H195" s="1"/>
-      <c r="V195" s="58"/>
+      <c r="V195" s="62"/>
     </row>
     <row r="196" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
@@ -7520,7 +7528,7 @@
       </c>
       <c r="E196"/>
       <c r="H196" s="1"/>
-      <c r="V196" s="58"/>
+      <c r="V196" s="62"/>
     </row>
     <row r="197" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
@@ -7537,7 +7545,7 @@
       </c>
       <c r="E197"/>
       <c r="H197" s="1"/>
-      <c r="V197" s="58"/>
+      <c r="V197" s="62"/>
     </row>
     <row r="198" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
@@ -7554,7 +7562,7 @@
       </c>
       <c r="E198"/>
       <c r="H198" s="1"/>
-      <c r="V198" s="58"/>
+      <c r="V198" s="62"/>
     </row>
     <row r="199" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
@@ -7571,7 +7579,7 @@
       </c>
       <c r="E199"/>
       <c r="H199" s="1"/>
-      <c r="V199" s="58"/>
+      <c r="V199" s="62"/>
     </row>
     <row r="200" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
@@ -7588,7 +7596,7 @@
       </c>
       <c r="E200"/>
       <c r="H200" s="1"/>
-      <c r="V200" s="58"/>
+      <c r="V200" s="62"/>
     </row>
     <row r="201" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
@@ -7605,7 +7613,7 @@
       </c>
       <c r="E201"/>
       <c r="H201" s="1"/>
-      <c r="V201" s="58"/>
+      <c r="V201" s="62"/>
     </row>
     <row r="202" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
@@ -7622,7 +7630,7 @@
       </c>
       <c r="E202"/>
       <c r="H202" s="1"/>
-      <c r="V202" s="58"/>
+      <c r="V202" s="62"/>
     </row>
     <row r="203" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
@@ -7639,7 +7647,7 @@
       </c>
       <c r="E203"/>
       <c r="H203" s="1"/>
-      <c r="V203" s="58"/>
+      <c r="V203" s="62"/>
     </row>
     <row r="204" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
@@ -7656,7 +7664,7 @@
       </c>
       <c r="E204"/>
       <c r="H204" s="1"/>
-      <c r="V204" s="58"/>
+      <c r="V204" s="62"/>
     </row>
     <row r="205" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
@@ -7673,7 +7681,7 @@
       </c>
       <c r="E205"/>
       <c r="H205" s="1"/>
-      <c r="V205" s="58"/>
+      <c r="V205" s="62"/>
     </row>
     <row r="206" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
@@ -7690,7 +7698,7 @@
       </c>
       <c r="E206"/>
       <c r="H206" s="1"/>
-      <c r="V206" s="58"/>
+      <c r="V206" s="62"/>
     </row>
     <row r="207" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
@@ -7707,7 +7715,7 @@
       </c>
       <c r="E207"/>
       <c r="H207" s="1"/>
-      <c r="V207" s="58"/>
+      <c r="V207" s="62"/>
     </row>
     <row r="208" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
@@ -7724,7 +7732,7 @@
       </c>
       <c r="E208"/>
       <c r="H208" s="1"/>
-      <c r="V208" s="58"/>
+      <c r="V208" s="62"/>
     </row>
     <row r="209" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
@@ -7741,7 +7749,7 @@
       </c>
       <c r="E209"/>
       <c r="H209" s="1"/>
-      <c r="V209" s="58"/>
+      <c r="V209" s="62"/>
     </row>
     <row r="210" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
@@ -7758,7 +7766,7 @@
       </c>
       <c r="E210"/>
       <c r="H210" s="1"/>
-      <c r="V210" s="58"/>
+      <c r="V210" s="62"/>
     </row>
     <row r="211" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
@@ -7775,7 +7783,7 @@
       </c>
       <c r="E211"/>
       <c r="H211" s="1"/>
-      <c r="V211" s="58"/>
+      <c r="V211" s="62"/>
     </row>
     <row r="212" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
@@ -7792,7 +7800,7 @@
       </c>
       <c r="E212"/>
       <c r="H212" s="1"/>
-      <c r="V212" s="58"/>
+      <c r="V212" s="62"/>
     </row>
     <row r="213" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
@@ -7809,7 +7817,7 @@
       </c>
       <c r="E213"/>
       <c r="H213" s="1"/>
-      <c r="V213" s="58"/>
+      <c r="V213" s="62"/>
     </row>
     <row r="214" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
@@ -7826,7 +7834,7 @@
       </c>
       <c r="E214"/>
       <c r="H214" s="1"/>
-      <c r="V214" s="58"/>
+      <c r="V214" s="62"/>
     </row>
     <row r="215" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
@@ -7843,7 +7851,7 @@
       </c>
       <c r="E215"/>
       <c r="H215" s="1"/>
-      <c r="V215" s="58"/>
+      <c r="V215" s="62"/>
     </row>
     <row r="216" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
@@ -7860,7 +7868,7 @@
       </c>
       <c r="E216"/>
       <c r="H216" s="1"/>
-      <c r="V216" s="58"/>
+      <c r="V216" s="62"/>
     </row>
     <row r="217" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
@@ -7877,7 +7885,7 @@
       </c>
       <c r="E217"/>
       <c r="H217" s="1"/>
-      <c r="V217" s="58"/>
+      <c r="V217" s="62"/>
     </row>
     <row r="218" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
@@ -7894,7 +7902,7 @@
       </c>
       <c r="E218"/>
       <c r="H218" s="1"/>
-      <c r="V218" s="58"/>
+      <c r="V218" s="62"/>
     </row>
     <row r="219" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
@@ -7911,7 +7919,7 @@
       </c>
       <c r="E219"/>
       <c r="H219" s="1"/>
-      <c r="V219" s="58"/>
+      <c r="V219" s="62"/>
     </row>
     <row r="220" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
@@ -7928,7 +7936,7 @@
       </c>
       <c r="E220"/>
       <c r="H220" s="1"/>
-      <c r="V220" s="58"/>
+      <c r="V220" s="62"/>
     </row>
     <row r="221" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
@@ -7945,7 +7953,7 @@
       </c>
       <c r="E221"/>
       <c r="H221" s="1"/>
-      <c r="V221" s="58"/>
+      <c r="V221" s="62"/>
     </row>
     <row r="222" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
@@ -7962,7 +7970,7 @@
       </c>
       <c r="E222"/>
       <c r="H222" s="1"/>
-      <c r="V222" s="58"/>
+      <c r="V222" s="62"/>
     </row>
     <row r="223" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
@@ -7984,6 +7992,7 @@
       <c r="N223">
         <v>1</v>
       </c>
+      <c r="V223" s="62"/>
     </row>
     <row r="224" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
@@ -7999,8 +8008,9 @@
         <v>1.2</v>
       </c>
       <c r="E224"/>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="V224" s="62"/>
+    </row>
+    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>3</v>
       </c>
@@ -8014,8 +8024,9 @@
         <v>1.2</v>
       </c>
       <c r="E225"/>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="V225" s="62"/>
+    </row>
+    <row r="226" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>3</v>
       </c>
@@ -8029,8 +8040,9 @@
         <v>1.2</v>
       </c>
       <c r="E226"/>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="V226" s="62"/>
+    </row>
+    <row r="227" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>3</v>
       </c>
@@ -8044,8 +8056,9 @@
         <v>1.2</v>
       </c>
       <c r="E227"/>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="V227" s="62"/>
+    </row>
+    <row r="228" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>3</v>
       </c>
@@ -8059,8 +8072,9 @@
         <v>1.2</v>
       </c>
       <c r="E228"/>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="V228" s="62"/>
+    </row>
+    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>3</v>
       </c>
@@ -8075,7 +8089,7 @@
       </c>
       <c r="E229"/>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>3</v>
       </c>
@@ -8090,7 +8104,7 @@
       </c>
       <c r="E230"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>3</v>
       </c>
@@ -8105,7 +8119,7 @@
       </c>
       <c r="E231"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>3</v>
       </c>
@@ -8120,7 +8134,7 @@
       </c>
       <c r="E232"/>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>3</v>
       </c>
@@ -8135,7 +8149,7 @@
       </c>
       <c r="E233"/>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>3</v>
       </c>
@@ -8150,7 +8164,7 @@
       </c>
       <c r="E234"/>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>3</v>
       </c>
@@ -8165,7 +8179,7 @@
       </c>
       <c r="E235"/>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>3</v>
       </c>
@@ -8180,7 +8194,7 @@
       </c>
       <c r="E236"/>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>3</v>
       </c>
@@ -8195,7 +8209,7 @@
       </c>
       <c r="E237"/>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>3</v>
       </c>
@@ -8210,7 +8224,7 @@
       </c>
       <c r="E238"/>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>3</v>
       </c>
@@ -8225,7 +8239,7 @@
       </c>
       <c r="E239"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>3</v>
       </c>
@@ -13270,11 +13284,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
     <mergeCell ref="V135:V137"/>
     <mergeCell ref="V138:V140"/>
     <mergeCell ref="V141:V143"/>
     <mergeCell ref="V161:V163"/>
+    <mergeCell ref="V165:V228"/>
     <mergeCell ref="V23:V30"/>
     <mergeCell ref="V43:V54"/>
     <mergeCell ref="V78:V109"/>

</xml_diff>